<commit_message>
completed layout for transponder board
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rocketry\Payload Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DCDBB4-9268-4FB5-91F3-B4ABD6F7D4B1}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E6231-D77D-4CB7-B5BB-B421730AF049}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -135,9 +135,6 @@
     <t>PhotoTransistor</t>
   </si>
   <si>
-    <t>9 pin molex</t>
-  </si>
-  <si>
     <t>xbee patch antenna</t>
   </si>
   <si>
@@ -157,6 +154,15 @@
   </si>
   <si>
     <t>https://www.digikey.ca/products/en?keywords=931-1075-ND</t>
+  </si>
+  <si>
+    <t>VI0921550000G</t>
+  </si>
+  <si>
+    <t>9 pin terminal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/amphenol-anytek/VI0921550000G/609-3943-ND/2261377</t>
   </si>
 </sst>
 </file>
@@ -562,7 +568,7 @@
   <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,7 +650,7 @@
         <v>39.14</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
@@ -838,20 +844,29 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -860,7 +875,7 @@
         <v>5.79</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="0"/>
@@ -875,7 +890,7 @@
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -887,7 +902,7 @@
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -899,7 +914,7 @@
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -908,7 +923,7 @@
         <v>12.85</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
@@ -922,7 +937,7 @@
       </c>
       <c r="G24" s="8">
         <f>SUM(G3:G21)</f>
-        <v>250.32999999999996</v>
+        <v>253.42999999999995</v>
       </c>
     </row>
   </sheetData>
@@ -930,5 +945,6 @@
     <hyperlink ref="F9" r:id="rId1" xr:uid="{0980C98E-8F65-4132-80A4-CE5A34535A3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed instr and recovery components per Alexs review
Added IMU current limiting resistors
Moved the caps near J4 on instr
Swapped out phototransistor footprint
Flipped I2C silk screen on J1 recovery
Flipped GND and TX silk screen on J6 recovery
renamed strat to alt on recovery silk screen
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rocketry\Payload Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39E6231-D77D-4CB7-B5BB-B421730AF049}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A513D-94B4-4B99-892A-ADD1C8E6FD00}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -237,7 +237,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -249,6 +249,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -568,7 +569,7 @@
   <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +650,7 @@
       <c r="E5" s="3">
         <v>39.14</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G5" s="8">
@@ -874,7 +875,7 @@
       <c r="E17" s="3">
         <v>5.79</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="9" t="s">
         <v>42</v>
       </c>
       <c r="G17" s="8">
@@ -943,8 +944,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F9" r:id="rId1" xr:uid="{0980C98E-8F65-4132-80A4-CE5A34535A3C}"/>
+    <hyperlink ref="F17" r:id="rId2" xr:uid="{9C3765C7-43A7-42F6-A6C2-6873E7847A9E}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{448EDABE-F16E-4F95-A746-01BC8EF98242}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re-Exported Gerber files with .05mm solder mask clearance
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rocketry\Payload Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8751C12A-E82E-4B98-BF2D-AC710F4283DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFDCB6E-3C68-4A99-8A0E-BD22941DDC8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -147,9 +147,6 @@
     <t>https://www.adafruit.com/product/1781</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/products/en?keywords=602-1964-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/products/en?keywords=931-1075-ND</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>GF-124-0204</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/digi-international/XBP9B-XCUT-001/602-1295-ND/3043287</t>
+  </si>
+  <si>
+    <t>XBP9B-XCUT-001</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="B2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -690,12 +693,14 @@
         <v>8</v>
       </c>
       <c r="G4" s="8">
-        <f t="shared" ref="G4:G21" si="0">E4*D4</f>
+        <f t="shared" ref="G4:G10" si="0">E4*D4</f>
         <v>7.14</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
+      <c r="B5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
@@ -703,14 +708,14 @@
         <v>2</v>
       </c>
       <c r="E5" s="3">
-        <v>39.14</v>
+        <v>54.3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" si="0"/>
-        <v>78.28</v>
+        <v>108.6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -757,10 +762,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>32</v>
@@ -769,7 +774,7 @@
         <v>0.24</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="8">
         <f t="shared" si="0"/>
@@ -778,10 +783,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9">
         <v>16</v>
@@ -790,7 +795,7 @@
         <v>0.22</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="0"/>
@@ -799,10 +804,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10">
         <v>16</v>
@@ -811,7 +816,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
@@ -835,7 +840,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" ref="G11:G26" si="1">E11*D11</f>
+        <f t="shared" ref="G11:G23" si="1">E11*D11</f>
         <v>1.96</v>
       </c>
     </row>
@@ -942,7 +947,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -954,7 +959,7 @@
         <v>2.13</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="8">
         <f t="shared" si="1"/>
@@ -963,10 +968,10 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -975,7 +980,7 @@
         <v>3.1</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="1"/>
@@ -994,7 +999,7 @@
         <v>5.79</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="8">
         <f t="shared" si="1"/>
@@ -1010,7 +1015,7 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
@@ -1022,7 +1027,7 @@
         <v>0.9</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G21" s="8">
         <f t="shared" si="1"/>
@@ -1031,7 +1036,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>37</v>
@@ -1043,7 +1048,7 @@
         <v>1.79</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G22" s="8">
         <f t="shared" si="1"/>
@@ -1082,17 +1087,16 @@
       </c>
       <c r="G26" s="8">
         <f>SUM(G3:G23)</f>
-        <v>280.09000000000003</v>
+        <v>310.41000000000003</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{448EDABE-F16E-4F95-A746-01BC8EF98242}"/>
-    <hyperlink ref="F11" r:id="rId2" xr:uid="{7E264208-5765-496E-A3EE-328632FA80F3}"/>
-    <hyperlink ref="F19" r:id="rId3" display="https://www.digikey.ca/products/en?keywords=602-1964-ND" xr:uid="{818F996A-5527-4DD9-ACCB-8E6A9FCE011F}"/>
-    <hyperlink ref="F23" r:id="rId4" xr:uid="{F793E299-D51A-404A-B688-2EF227C857CA}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{7E264208-5765-496E-A3EE-328632FA80F3}"/>
+    <hyperlink ref="F19" r:id="rId2" display="https://www.digikey.ca/products/en?keywords=602-1964-ND" xr:uid="{818F996A-5527-4DD9-ACCB-8E6A9FCE011F}"/>
+    <hyperlink ref="F23" r:id="rId3" xr:uid="{F793E299-D51A-404A-B688-2EF227C857CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added zips for gerber files
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rocketry\Payload Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFDCB6E-3C68-4A99-8A0E-BD22941DDC8A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EBDEEE-B591-445E-BD36-F032FFF7EA78}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -208,6 +208,36 @@
   </si>
   <si>
     <t>XBP9B-XCUT-001</t>
+  </si>
+  <si>
+    <t>PPPC051LFBN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC051LFBN-RC/S7038-ND/810177</t>
+  </si>
+  <si>
+    <t>5 position female header</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC101LFBN-RC/S7008-ND/810149</t>
+  </si>
+  <si>
+    <t>10 position female header</t>
+  </si>
+  <si>
+    <t>PPTC101LFBN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/NPPN101BFCN-RC/S5751-10-ND/804812</t>
+  </si>
+  <si>
+    <t>10 position xbee header</t>
+  </si>
+  <si>
+    <t>NPPN101BFCN-RC</t>
+  </si>
+  <si>
+    <t>Right angle JST-PH</t>
   </si>
 </sst>
 </file>
@@ -289,7 +319,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -300,7 +330,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -622,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9A9FBE-909F-48F5-B518-221EFB836478}">
-  <dimension ref="B2:G26"/>
+  <dimension ref="B2:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,6 +664,7 @@
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.77734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="25.77734375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
@@ -653,12 +683,12 @@
       <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -671,13 +701,13 @@
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="3">
         <f>E3*D3</f>
         <v>17.98</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -692,7 +722,7 @@
       <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G10" si="0">E4*D4</f>
         <v>7.14</v>
       </c>
@@ -713,13 +743,13 @@
       <c r="F5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>108.6</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
@@ -734,13 +764,13 @@
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>11.129999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
@@ -755,13 +785,13 @@
       <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>6.6000000000000005</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C8" t="s">
@@ -776,13 +806,13 @@
       <c r="F8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>7.68</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C9" t="s">
@@ -797,13 +827,13 @@
       <c r="F9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>3.52</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>52</v>
       </c>
       <c r="C10" t="s">
@@ -818,13 +848,13 @@
       <c r="F10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
@@ -839,13 +869,13 @@
       <c r="F11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="8">
-        <f t="shared" ref="G11:G23" si="1">E11*D11</f>
+      <c r="G11" s="3">
+        <f t="shared" ref="G11:G26" si="1">E11*D11</f>
         <v>1.96</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C12" t="s">
@@ -860,13 +890,13 @@
       <c r="F12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="3">
         <f t="shared" si="1"/>
         <v>2.64</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="10"/>
+      <c r="B13" s="9"/>
       <c r="C13" t="s">
         <v>24</v>
       </c>
@@ -879,13 +909,13 @@
       <c r="F13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>19.36</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="10"/>
+      <c r="B14" s="9"/>
       <c r="C14" t="s">
         <v>25</v>
       </c>
@@ -898,13 +928,13 @@
       <c r="F14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>51.58</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
@@ -919,13 +949,13 @@
       <c r="F15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="3">
         <f t="shared" si="1"/>
         <v>4.42</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
       <c r="C16" t="s">
@@ -940,13 +970,13 @@
       <c r="F16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="3">
         <f t="shared" si="1"/>
         <v>11.96</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C17" t="s">
@@ -961,13 +991,13 @@
       <c r="F17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="3">
         <f t="shared" si="1"/>
         <v>4.26</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C18" t="s">
@@ -982,13 +1012,13 @@
       <c r="F18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="3">
         <f t="shared" si="1"/>
         <v>3.1</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
       <c r="C19" t="s">
         <v>35</v>
       </c>
@@ -998,17 +1028,20 @@
       <c r="E19" s="3">
         <v>5.79</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="3">
         <f t="shared" si="1"/>
         <v>11.58</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="10"/>
-      <c r="G20" s="8">
+      <c r="B20" s="9"/>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1029,7 +1062,7 @@
       <c r="F21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="3">
         <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
@@ -1050,13 +1083,13 @@
       <c r="F22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="3">
         <f t="shared" si="1"/>
         <v>7.16</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="10"/>
+      <c r="B23" s="9"/>
       <c r="C23" t="s">
         <v>38</v>
       </c>
@@ -1069,25 +1102,81 @@
       <c r="F23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="3">
         <f t="shared" si="1"/>
         <v>25.7</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.68</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="1"/>
+        <v>6.12</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
+      <c r="B25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="1"/>
+        <v>10.8</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="3" t="e">
-        <f>G2Total</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G26" s="8">
-        <f>SUM(G3:G23)</f>
-        <v>310.41000000000003</v>
+      <c r="B26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1.36</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="3">
+        <f t="shared" si="1"/>
+        <v>8.16</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="3">
+        <f>SUM(G3:G26)</f>
+        <v>335.49000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
restucture of recovery code for new comm standard
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rocketry\Payload Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DC8CE8-912A-406E-B9BD-EFB7C3ECB9FA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904E744C-2D2C-4B69-813C-D4A3E28B115E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9048" xr2:uid="{01722910-1F74-43C0-9D12-5EE3A1FCE81D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
   <dimension ref="B2:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,7 +902,7 @@
       <c r="E6" s="3">
         <v>3.71</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3">
@@ -1654,8 +1654,9 @@
     <hyperlink ref="F40" r:id="rId2" xr:uid="{D3385668-B9E8-4C64-A6FB-609982F2DD1E}"/>
     <hyperlink ref="F9" r:id="rId3" xr:uid="{E393362D-78C3-406D-88CB-B8F0B37A0E3B}"/>
     <hyperlink ref="F26" r:id="rId4" xr:uid="{0C5990B7-BBE1-4BFA-BD84-F845E253B1BA}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{3822E11F-082B-4E28-A4D1-362AF8A7A7D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>